<commit_message>
feat: additional validation rule examples
</commit_message>
<xml_diff>
--- a/support/tabular-assurance/test-results/assurance-issues.xlsx
+++ b/support/tabular-assurance/test-results/assurance-issues.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>session_id</t>
   </si>
@@ -33,7 +33,7 @@
     <t>remediation</t>
   </si>
   <si>
-    <t>91cddd36-603e-43fd-a265-70bd56024a18</t>
+    <t>b064392b-217a-4b17-9893-fc301ca6f256</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -136,6 +136,27 @@
   </si>
   <si>
     <t>Provide a value for column7</t>
+  </si>
+  <si>
+    <t>Pattern Mismatch</t>
+  </si>
+  <si>
+    <t>column8</t>
+  </si>
+  <si>
+    <t>ABC-ABCD</t>
+  </si>
+  <si>
+    <t>Value ABC-ABCD in column8 does not match the pattern ABC-1234</t>
+  </si>
+  <si>
+    <t>Follow the pattern ABC-1234 in column8</t>
+  </si>
+  <si>
+    <t>XYZ-1234</t>
+  </si>
+  <si>
+    <t>Value XYZ-1234 in column8 does not match the pattern ABC-1234</t>
   </si>
 </sst>
 </file>
@@ -540,6 +561,75 @@
         <v>41</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>